<commit_message>
SQL approach to data selectors
</commit_message>
<xml_diff>
--- a/Suburb Locality.xlsx
+++ b/Suburb Locality.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20376"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\ad.police.wa.gov.au\Shares\OrgUnits\S\StratPerformance\General\OPEU\Work\Tasks\2021\SPRA-7225 University Engagements\SPRA-7226 Capstone Projects UWA\Capstone Projects\Open Source Data Projects\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1689a769bbf24956/Uni/CITS3200/WA-Crime/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{444B4E3D-424D-4938-B9F4-6560308126EF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="18" documentId="8_{444B4E3D-424D-4938-B9F4-6560308126EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8C8BF99B-2D07-4FAB-963E-5FC0D7464FDE}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18870" windowHeight="10335" xr2:uid="{A6747452-0587-4896-809C-9A5BBF7E55FE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{A6747452-0587-4896-809C-9A5BBF7E55FE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14132" uniqueCount="3555">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14149" uniqueCount="3559">
   <si>
     <t>SUB_TXT</t>
   </si>
@@ -10690,6 +10690,18 @@
   </si>
   <si>
     <t>ZUYTDORP</t>
+  </si>
+  <si>
+    <t>&lt;--</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
   </si>
 </sst>
 </file>
@@ -11042,9 +11054,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17E1E123-FC4F-4246-884B-7DD9953BB53D}">
-  <dimension ref="A1:D3533"/>
+  <dimension ref="A1:M3533"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M4" sqref="M4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -11054,7 +11068,7 @@
     <col min="4" max="4" width="29.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -11067,8 +11081,11 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -11081,8 +11098,26 @@
       <c r="D2" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I2">
+        <v>1000</v>
+      </c>
+      <c r="J2" t="s">
+        <v>3555</v>
+      </c>
+      <c r="K2" t="s">
+        <v>3555</v>
+      </c>
+      <c r="L2" t="s">
+        <v>3556</v>
+      </c>
+      <c r="M2">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
@@ -11095,8 +11130,20 @@
       <c r="D3" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I3">
+        <v>250</v>
+      </c>
+      <c r="L3" t="s">
+        <v>3557</v>
+      </c>
+      <c r="M3">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
@@ -11109,8 +11156,20 @@
       <c r="D4" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I4">
+        <v>300</v>
+      </c>
+      <c r="L4" t="s">
+        <v>3558</v>
+      </c>
+      <c r="M4">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
@@ -11123,8 +11182,14 @@
       <c r="D5" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I5">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>13</v>
       </c>
@@ -11137,8 +11202,11 @@
       <c r="D6" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H6" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>16</v>
       </c>
@@ -11151,8 +11219,11 @@
       <c r="D7" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H7" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>19</v>
       </c>
@@ -11165,8 +11236,11 @@
       <c r="D8" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H8" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>22</v>
       </c>
@@ -11179,8 +11253,11 @@
       <c r="D9" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H9" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>25</v>
       </c>
@@ -11193,8 +11270,11 @@
       <c r="D10" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H10" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>27</v>
       </c>
@@ -11207,8 +11287,11 @@
       <c r="D11" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H11" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>29</v>
       </c>
@@ -11221,8 +11304,11 @@
       <c r="D12" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H12" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>31</v>
       </c>
@@ -11236,7 +11322,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>33</v>
       </c>
@@ -11250,7 +11336,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>34</v>
       </c>
@@ -11263,8 +11349,9 @@
       <c r="D15" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H15" s="1"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>36</v>
       </c>
@@ -11277,8 +11364,9 @@
       <c r="D16" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H16" s="1"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>38</v>
       </c>
@@ -11291,8 +11379,9 @@
       <c r="D17" s="1" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H17" s="1"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>42</v>
       </c>
@@ -11305,8 +11394,9 @@
       <c r="D18" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H18" s="1"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>44</v>
       </c>
@@ -11319,8 +11409,9 @@
       <c r="D19" s="1" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H19" s="1"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>48</v>
       </c>
@@ -11333,8 +11424,9 @@
       <c r="D20" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H20" s="1"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>50</v>
       </c>
@@ -11347,8 +11439,9 @@
       <c r="D21" s="1" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H21" s="1"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>52</v>
       </c>
@@ -11361,8 +11454,9 @@
       <c r="D22" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H22" s="1"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>54</v>
       </c>
@@ -11375,8 +11469,9 @@
       <c r="D23" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H23" s="1"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>56</v>
       </c>
@@ -11389,8 +11484,9 @@
       <c r="D24" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H24" s="1"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>57</v>
       </c>
@@ -11403,8 +11499,9 @@
       <c r="D25" s="1" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H25" s="1"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>59</v>
       </c>
@@ -11417,8 +11514,9 @@
       <c r="D26" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H26" s="1"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>61</v>
       </c>
@@ -11431,8 +11529,9 @@
       <c r="D27" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H27" s="1"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>63</v>
       </c>
@@ -11445,8 +11544,9 @@
       <c r="D28" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H28" s="1"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>64</v>
       </c>
@@ -11459,8 +11559,9 @@
       <c r="D29" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H29" s="1"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>66</v>
       </c>
@@ -11473,8 +11574,9 @@
       <c r="D30" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H30" s="1"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>68</v>
       </c>
@@ -11487,8 +11589,9 @@
       <c r="D31" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H31" s="1"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>71</v>
       </c>
@@ -11501,6 +11604,7 @@
       <c r="D32" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="H32" s="1"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">

</xml_diff>